<commit_message>
building sample type from less well-formed spreadsheet
futher test cases and code cleaning
</commit_message>
<xml_diff>
--- a/test/fixtures/files/sample-type-example.xlsx
+++ b/test/fixtures/files/sample-type-example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>some stuff</t>
   </si>
@@ -369,15 +369,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -391,7 +396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>